<commit_message>
fixed lock release issue when Excel file is corrupt.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Item</t>
   </si>
@@ -146,28 +146,34 @@
     <t>Hi, Avner!</t>
   </si>
   <si>
+    <t>appPackage</t>
+  </si>
+  <si>
+    <t>Avner</t>
+  </si>
+  <si>
+    <t>MobileOS</t>
+  </si>
+  <si>
+    <t>ShirNate</t>
+  </si>
+  <si>
+    <t>Galaxy S5 SM-G900A</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>johndoe@perfectomobile.com</t>
+  </si>
+  <si>
+    <t>yyyyy</t>
+  </si>
+  <si>
+    <t>Hi, John!</t>
+  </si>
+  <si>
     <t>a1001a</t>
-  </si>
-  <si>
-    <t>appPackage</t>
-  </si>
-  <si>
-    <t>dudu@gulu.com</t>
-  </si>
-  <si>
-    <t>Hi, Mister!</t>
-  </si>
-  <si>
-    <t>Avner</t>
-  </si>
-  <si>
-    <t>MobileOS</t>
-  </si>
-  <si>
-    <t>ShirNate</t>
-  </si>
-  <si>
-    <t>Galaxy S5 SM-G900A</t>
   </si>
 </sst>
 </file>
@@ -513,27 +519,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -568,40 +574,40 @@
         <v>29</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E2" t="s">
         <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E3" t="s">
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -614,18 +620,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -636,23 +642,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -672,14 +681,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" width="16.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.1328125" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -701,7 +710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -712,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -737,15 +746,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" width="14.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.1328125" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -756,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -767,7 +776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -778,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added support for IE and FF. Added try for driver creation, to avoid failure of the beforeMetod.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080"/>
   </bookViews>
   <sheets>
-    <sheet name="devices" sheetId="11" r:id="rId1"/>
+    <sheet name="devices" sheetId="19" r:id="rId1"/>
     <sheet name="signIn" sheetId="18" r:id="rId2"/>
     <sheet name="items" sheetId="1" r:id="rId3"/>
     <sheet name="addresses" sheetId="7" r:id="rId4"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Item</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>a1001a</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>iexplorer</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -605,6 +614,21 @@
       </c>
       <c r="J4" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for full detailed excel report
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="devices" sheetId="19" r:id="rId1"/>
-    <sheet name="signIn" sheetId="18" r:id="rId2"/>
-    <sheet name="items" sheetId="1" r:id="rId3"/>
-    <sheet name="addresses" sheetId="7" r:id="rId4"/>
+    <sheet name="devices (2)" sheetId="20" r:id="rId1"/>
+    <sheet name="devices" sheetId="19" r:id="rId2"/>
+    <sheet name="signIn" sheetId="18" r:id="rId3"/>
+    <sheet name="items" sheetId="1" r:id="rId4"/>
+    <sheet name="addresses" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Item</t>
   </si>
@@ -173,13 +174,10 @@
     <t>a1001a</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>iexplorer</t>
-  </si>
-  <si>
-    <t>firefox</t>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -523,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -626,11 +624,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -638,6 +631,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -694,7 +760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -759,7 +825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
* Screenshots folder name changed to be taken from properties file. * Fixed folder names to be cross browser compatible.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avner/git/Beton/Beton/src/main/resources/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices (2)" sheetId="20" r:id="rId1"/>
@@ -18,9 +18,12 @@
     <sheet name="items" sheetId="1" r:id="rId4"/>
     <sheet name="addresses" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Item</t>
   </si>
@@ -527,23 +530,23 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -581,7 +584,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>31</v>
       </c>
@@ -592,7 +595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>31</v>
       </c>
@@ -603,7 +606,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>43</v>
       </c>
@@ -614,12 +617,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -635,26 +638,26 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -692,9 +695,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>48</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -711,14 +717,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -729,7 +735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
@@ -740,7 +746,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>44</v>
       </c>
@@ -768,14 +774,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.1328125" style="2" collapsed="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.1640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -797,7 +803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -808,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -833,15 +839,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.73046875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.1328125" style="2" collapsed="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.1640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -852,7 +858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -863,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -874,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
* Added support for screenshots in detailed report. * Moved testCycle param from xml to properties file.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Item</t>
   </si>
@@ -635,10 +635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -701,6 +701,11 @@
       </c>
       <c r="J2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed properties file + fixed locking issue with Excel file, when pointer is null.
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices (2)" sheetId="20" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>deviceName</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -627,11 +627,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -642,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added support for encrypted password. In order to use encryption, add "~" prefix to the password in the properties file
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>deviceName</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>beton.yatsuk@gmail.com</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Appium</t>
+  </si>
+  <si>
+    <t>testssts</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,11 +629,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed screenshot links compatibility issues with Windows/Linux
</commit_message>
<xml_diff>
--- a/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/Beton/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avner/git/Beton/Beton/src/main/resources/dataSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices (2)" sheetId="20" r:id="rId1"/>
@@ -18,18 +18,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>deviceName</t>
   </si>
@@ -116,12 +116,6 @@
   </si>
   <si>
     <t>Android</t>
-  </si>
-  <si>
-    <t>Appium</t>
-  </si>
-  <si>
-    <t>testssts</t>
   </si>
 </sst>
 </file>
@@ -463,23 +457,23 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>11</v>
       </c>
@@ -528,7 +522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>11</v>
       </c>
@@ -539,7 +533,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>20</v>
       </c>
@@ -550,12 +544,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -571,26 +565,26 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>28</v>
       </c>
@@ -637,12 +631,6 @@
       </c>
       <c r="J2" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -659,14 +647,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -677,7 +665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -688,7 +676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>